<commit_message>
Deploying to gh-pages from @ Open-Systems-Pharmacology/OSPSuite.ReportingEngine@f7527aff9a24fa8ee28eb4e481944f2276f568e3 🚀
</commit_message>
<xml_diff>
--- a/docs/dev/articles/templates/WorkflowInput.xlsx
+++ b/docs/dev/articles/templates/WorkflowInput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.ReportingEngine\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4E628B-3D09-427D-86C7-71105F3B5A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6244981-9F1B-4280-9D87-79CDA783064A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="914" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="914" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -1504,9 +1504,6 @@
     <t>FEMALE</t>
   </si>
   <si>
-    <t>Make sure 1=male 2= female</t>
-  </si>
-  <si>
     <t>ALL</t>
   </si>
   <si>
@@ -1751,6 +1748,9 @@
   </si>
   <si>
     <t xml:space="preserve">Path to the mass balance settings (json) RELATIVE to workflow.R, e.g. mass-balance-settings.json or Models/mass-balance-settings.json </t>
+  </si>
+  <si>
+    <t>Make sure male="MALE" and female="FEMALE"</t>
   </si>
 </sst>
 </file>
@@ -1967,6 +1967,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF5050FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFCE3D32"/>
         </patternFill>
       </fill>
@@ -2024,13 +2031,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF466983"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5050FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2609,8 +2609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2628,10 +2628,10 @@
         <v>52</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>413</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>414</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>0</v>
@@ -2826,7 +2826,7 @@
         <v>91</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>360</v>
+        <v>417</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -3039,7 +3039,7 @@
         <v>332</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -3080,7 +3080,7 @@
         <v>333</v>
       </c>
       <c r="M2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -3121,7 +3121,7 @@
         <v>334</v>
       </c>
       <c r="M3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -3147,7 +3147,7 @@
         <v>335</v>
       </c>
       <c r="M4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -3170,7 +3170,7 @@
         <v>336</v>
       </c>
       <c r="M5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -3190,7 +3190,7 @@
         <v>337</v>
       </c>
       <c r="M6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -3210,7 +3210,7 @@
         <v>340</v>
       </c>
       <c r="M7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -3230,7 +3230,7 @@
         <v>338</v>
       </c>
       <c r="M8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -3250,7 +3250,7 @@
         <v>339</v>
       </c>
       <c r="M9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -3264,7 +3264,7 @@
         <v>200</v>
       </c>
       <c r="M10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -3278,7 +3278,7 @@
         <v>235</v>
       </c>
       <c r="M11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -3292,7 +3292,7 @@
         <v>270</v>
       </c>
       <c r="M12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -3306,7 +3306,7 @@
         <v>23</v>
       </c>
       <c r="M13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -3320,7 +3320,7 @@
         <v>24</v>
       </c>
       <c r="M14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -3334,7 +3334,7 @@
         <v>271</v>
       </c>
       <c r="M15" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -3348,7 +3348,7 @@
         <v>272</v>
       </c>
       <c r="M16" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="17" spans="5:13" x14ac:dyDescent="0.2">
@@ -3362,7 +3362,7 @@
         <v>25</v>
       </c>
       <c r="M17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="18" spans="5:13" x14ac:dyDescent="0.2">
@@ -3376,7 +3376,7 @@
         <v>273</v>
       </c>
       <c r="M18" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="19" spans="5:13" x14ac:dyDescent="0.2">
@@ -3390,7 +3390,7 @@
         <v>26</v>
       </c>
       <c r="M19" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="20" spans="5:13" x14ac:dyDescent="0.2">
@@ -3404,7 +3404,7 @@
         <v>29</v>
       </c>
       <c r="M20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="21" spans="5:13" x14ac:dyDescent="0.2">
@@ -3418,7 +3418,7 @@
         <v>31</v>
       </c>
       <c r="M21" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="22" spans="5:13" x14ac:dyDescent="0.2">
@@ -3432,7 +3432,7 @@
         <v>274</v>
       </c>
       <c r="M22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="23" spans="5:13" x14ac:dyDescent="0.2">
@@ -3570,7 +3570,7 @@
         <v>100</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>105</v>
@@ -3600,10 +3600,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>379</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>380</v>
       </c>
       <c r="C5" s="15"/>
     </row>
@@ -3612,7 +3612,7 @@
         <v>331</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C6" s="15"/>
     </row>
@@ -3621,7 +3621,7 @@
         <v>131</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>109</v>
@@ -3629,10 +3629,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>366</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>367</v>
       </c>
       <c r="C8" s="15"/>
     </row>
@@ -3970,7 +3970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
@@ -4018,21 +4018,21 @@
         <v>4</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
+        <v>381</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>382</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
@@ -4040,13 +4040,13 @@
         <v>285</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4120,7 +4120,7 @@
         <v>310</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>110</v>
@@ -4134,7 +4134,7 @@
         <v>324</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>110</v>
@@ -4170,7 +4170,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="29" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
@@ -4178,10 +4178,10 @@
     </row>
     <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>415</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -4318,32 +4318,32 @@
     </row>
     <row r="5" spans="1:4" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
+        <v>376</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>377</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="18" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
+        <v>384</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>411</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>385</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>412</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="18" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
@@ -4351,13 +4351,13 @@
         <v>285</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
@@ -4371,15 +4371,15 @@
         <v>328</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
+        <v>367</v>
+      </c>
+      <c r="B10" s="24" t="s">
         <v>368</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>369</v>
       </c>
       <c r="C10" s="21"/>
     </row>
@@ -4432,35 +4432,35 @@
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"#BA6338"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="87" operator="equal">
-      <formula>"#5050FF"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="78" operator="equal">
       <formula>"#466983"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="79" operator="equal">
       <formula>"green"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="80" operator="equal">
       <formula>"yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="81" operator="equal">
       <formula>"blue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="82" operator="equal">
       <formula>"red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="83" operator="equal">
       <formula>"black"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="84" operator="equal">
       <formula>"#F0E685"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="85" operator="equal">
       <formula>"#749B58"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="86" operator="equal">
       <formula>"#CE3D32"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="87" operator="equal">
+      <formula>"#5050FF"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4507,15 +4507,15 @@
         <v>2</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>374</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>295</v>
@@ -4551,10 +4551,10 @@
     </row>
     <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Open-Systems-Pharmacology/OSPSuite.ReportingEngine@252a1667c9e5c8ee8ce6d30702646d25f1ab6f45 🚀
</commit_message>
<xml_diff>
--- a/docs/dev/articles/templates/WorkflowInput.xlsx
+++ b/docs/dev/articles/templates/WorkflowInput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design2Code\OSPSuite.ReportingEngine\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierre Chelle\Documents\Design2Code\OSPSuite.ReportingEngine\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6244981-9F1B-4280-9D87-79CDA783064A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837E7BE3-612B-4C2C-885D-28F9B403B082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="914" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="914" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="12" r:id="rId1"/>
@@ -25,15 +25,16 @@
     <sheet name="PK Fraction" sheetId="19" r:id="rId10"/>
     <sheet name="SensitivityParameter" sheetId="7" r:id="rId11"/>
     <sheet name="tpDictionary" sheetId="11" r:id="rId12"/>
-    <sheet name="StudyDesign" sheetId="21" r:id="rId13"/>
-    <sheet name="Lookup" sheetId="16" r:id="rId14"/>
+    <sheet name="tpDictionaryLoq" sheetId="23" r:id="rId13"/>
+    <sheet name="StudyDesign" sheetId="21" r:id="rId14"/>
+    <sheet name="Lookup" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="418">
   <si>
     <t>reportName</t>
   </si>
@@ -1889,7 +1890,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1959,6 +1960,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2499,12 +2502,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.125" customWidth="1"/>
+    <col min="1" max="1" width="20.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>93</v>
       </c>
@@ -2512,7 +2515,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>94</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>95</v>
       </c>
@@ -2540,13 +2543,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>158</v>
       </c>
@@ -2557,12 +2560,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2579,22 +2582,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>317</v>
       </c>
@@ -2607,20 +2610,20 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="48.125" customWidth="1"/>
+    <col min="7" max="7" width="48.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>318</v>
       </c>
@@ -2643,7 +2646,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>54</v>
       </c>
@@ -2658,7 +2661,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>57</v>
       </c>
@@ -2673,7 +2676,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>59</v>
       </c>
@@ -2690,7 +2693,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>62</v>
       </c>
@@ -2707,7 +2710,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>65</v>
       </c>
@@ -2724,7 +2727,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>69</v>
       </c>
@@ -2745,7 +2748,7 @@
       </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>75</v>
       </c>
@@ -2766,7 +2769,7 @@
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>80</v>
       </c>
@@ -2787,7 +2790,7 @@
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>85</v>
       </c>
@@ -2808,7 +2811,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>89</v>
       </c>
@@ -2827,23 +2830,6 @@
       </c>
       <c r="G11" s="9" t="s">
         <v>417</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2853,20 +2839,270 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05B762A-0A3E-4AE3-9238-C14EE5C34AFE}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.4140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>318</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>413</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="32"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="32"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="32"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="32"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.375" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="18.25" customWidth="1"/>
-    <col min="3" max="3" width="19.125" customWidth="1"/>
+    <col min="3" max="3" width="19.08203125" customWidth="1"/>
     <col min="4" max="4" width="40.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>79</v>
       </c>
@@ -2880,7 +3116,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>77</v>
       </c>
@@ -2892,7 +3128,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>354</v>
       </c>
@@ -2906,7 +3142,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>20</v>
       </c>
@@ -2920,7 +3156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>20</v>
       </c>
@@ -2934,7 +3170,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>40</v>
       </c>
@@ -2948,7 +3184,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>40</v>
       </c>
@@ -2962,7 +3198,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>60</v>
       </c>
@@ -2978,7 +3214,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:M37"/>
   <sheetViews>
@@ -2987,21 +3223,21 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.08203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>103</v>
       </c>
@@ -3042,7 +3278,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>105</v>
       </c>
@@ -3083,7 +3319,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -3124,7 +3360,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>107</v>
       </c>
@@ -3150,7 +3386,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
         <v>162</v>
       </c>
@@ -3173,7 +3409,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>163</v>
       </c>
@@ -3193,7 +3429,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
         <v>164</v>
       </c>
@@ -3213,7 +3449,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>165</v>
       </c>
@@ -3233,7 +3469,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
         <v>166</v>
       </c>
@@ -3253,7 +3489,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
         <v>167</v>
       </c>
@@ -3267,7 +3503,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>168</v>
       </c>
@@ -3281,7 +3517,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
         <v>169</v>
       </c>
@@ -3295,7 +3531,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
         <v>170</v>
       </c>
@@ -3309,7 +3545,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
         <v>171</v>
       </c>
@@ -3323,7 +3559,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
         <v>172</v>
       </c>
@@ -3337,7 +3573,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
         <v>173</v>
       </c>
@@ -3351,7 +3587,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="17" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
         <v>174</v>
       </c>
@@ -3365,7 +3601,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="18" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
         <v>175</v>
       </c>
@@ -3379,7 +3615,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="19" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
         <v>176</v>
       </c>
@@ -3393,7 +3629,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="20" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
         <v>177</v>
       </c>
@@ -3407,7 +3643,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="21" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
         <v>178</v>
       </c>
@@ -3421,7 +3657,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="22" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
         <v>179</v>
       </c>
@@ -3435,7 +3671,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="23" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>180</v>
       </c>
@@ -3443,7 +3679,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>181</v>
       </c>
@@ -3451,7 +3687,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
         <v>182</v>
       </c>
@@ -3459,7 +3695,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
         <v>183</v>
       </c>
@@ -3467,7 +3703,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="27" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E27" t="s">
         <v>184</v>
       </c>
@@ -3475,7 +3711,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="28" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E28" t="s">
         <v>185</v>
       </c>
@@ -3483,7 +3719,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="29" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
         <v>186</v>
       </c>
@@ -3491,42 +3727,42 @@
         <v>227</v>
       </c>
     </row>
-    <row r="30" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="5:13" x14ac:dyDescent="0.3">
       <c r="G30" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="31" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="5:13" x14ac:dyDescent="0.3">
       <c r="G31" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="5:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="5:13" x14ac:dyDescent="0.3">
       <c r="G32" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G33" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G35" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G36" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G37" t="s">
         <v>234</v>
       </c>
@@ -3546,7 +3782,7 @@
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="100.25" customWidth="1"/>
@@ -3554,7 +3790,7 @@
     <col min="6" max="6" width="22.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -3565,7 +3801,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="38" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>100</v>
       </c>
@@ -3576,7 +3812,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>101</v>
       </c>
@@ -3587,7 +3823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>129</v>
       </c>
@@ -3598,7 +3834,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>378</v>
       </c>
@@ -3607,7 +3843,7 @@
       </c>
       <c r="C5" s="15"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>331</v>
       </c>
@@ -3616,7 +3852,7 @@
       </c>
       <c r="C6" s="15"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>131</v>
       </c>
@@ -3627,7 +3863,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>365</v>
       </c>
@@ -3636,7 +3872,7 @@
       </c>
       <c r="C8" s="15"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>320</v>
       </c>
@@ -3645,14 +3881,14 @@
       </c>
       <c r="C9" s="15"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="s">
         <v>329</v>
       </c>
       <c r="B10" s="28"/>
       <c r="C10" s="28"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>111</v>
       </c>
@@ -3663,7 +3899,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>113</v>
       </c>
@@ -3674,7 +3910,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>115</v>
       </c>
@@ -3685,7 +3921,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>117</v>
       </c>
@@ -3696,7 +3932,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>119</v>
       </c>
@@ -3707,7 +3943,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>121</v>
       </c>
@@ -3718,7 +3954,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>123</v>
       </c>
@@ -3729,7 +3965,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>124</v>
       </c>
@@ -3740,7 +3976,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>125</v>
       </c>
@@ -3751,14 +3987,14 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="28" t="s">
         <v>330</v>
       </c>
       <c r="B20" s="28"/>
       <c r="C20" s="28"/>
     </row>
-    <row r="21" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="38.5" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>132</v>
       </c>
@@ -3767,7 +4003,7 @@
       </c>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
         <v>133</v>
       </c>
@@ -3778,7 +4014,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="51" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
         <v>137</v>
       </c>
@@ -3787,7 +4023,7 @@
       </c>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
         <v>138</v>
       </c>
@@ -3796,7 +4032,7 @@
       </c>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
         <v>140</v>
       </c>
@@ -3807,7 +4043,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
         <v>141</v>
       </c>
@@ -3816,7 +4052,7 @@
       </c>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="38" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
         <v>155</v>
       </c>
@@ -3825,7 +4061,7 @@
       </c>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
         <v>147</v>
       </c>
@@ -3834,7 +4070,7 @@
       </c>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
         <v>148</v>
       </c>
@@ -3843,7 +4079,7 @@
       </c>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
         <v>151</v>
       </c>
@@ -3852,7 +4088,7 @@
       </c>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
         <v>153</v>
       </c>
@@ -3861,14 +4097,14 @@
       </c>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
         <v>349</v>
       </c>
       <c r="B32" s="28"/>
       <c r="C32" s="28"/>
     </row>
-    <row r="33" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="51" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
         <v>350</v>
       </c>
@@ -3975,15 +4211,15 @@
       <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.875" customWidth="1"/>
-    <col min="2" max="2" width="42.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.75" customWidth="1"/>
     <col min="4" max="4" width="29.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
@@ -3997,7 +4233,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>291</v>
       </c>
@@ -4005,7 +4241,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="18" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="18" customFormat="1" ht="38.5" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>293</v>
       </c>
@@ -4013,7 +4249,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="18" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="18" customFormat="1" ht="38.5" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>4</v>
       </c>
@@ -4027,7 +4263,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="18" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>381</v>
       </c>
@@ -4035,7 +4271,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="18" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="18" customFormat="1" ht="75.5" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>285</v>
       </c>
@@ -4049,7 +4285,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>286</v>
       </c>
@@ -4063,7 +4299,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>303</v>
       </c>
@@ -4077,7 +4313,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>322</v>
       </c>
@@ -4091,7 +4327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>305</v>
       </c>
@@ -4099,7 +4335,7 @@
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
     </row>
-    <row r="11" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>306</v>
       </c>
@@ -4107,7 +4343,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>308</v>
       </c>
@@ -4115,7 +4351,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>310</v>
       </c>
@@ -4129,7 +4365,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="18" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="18" customFormat="1" ht="38" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>324</v>
       </c>
@@ -4143,7 +4379,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>311</v>
       </c>
@@ -4157,7 +4393,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="18" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" s="18" customFormat="1" ht="89" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>312</v>
       </c>
@@ -4168,7 +4404,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
         <v>414</v>
       </c>
@@ -4176,7 +4412,7 @@
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
     </row>
-    <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="38" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>415</v>
       </c>
@@ -4252,15 +4488,15 @@
       <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.75" style="6" customWidth="1"/>
-    <col min="2" max="2" width="30.625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="47.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.58203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
@@ -4274,7 +4510,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>283</v>
       </c>
@@ -4288,7 +4524,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>284</v>
       </c>
@@ -4302,7 +4538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>11</v>
       </c>
@@ -4316,7 +4552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="18" customFormat="1" ht="56" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>376</v>
       </c>
@@ -4324,7 +4560,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="18" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>383</v>
       </c>
@@ -4335,7 +4571,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="18" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="18" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>384</v>
       </c>
@@ -4346,7 +4582,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="18" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="18" customFormat="1" ht="140" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>285</v>
       </c>
@@ -4360,7 +4596,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="18" customFormat="1" ht="56" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>286</v>
       </c>
@@ -4374,7 +4610,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="18" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>367</v>
       </c>
@@ -4383,7 +4619,7 @@
       </c>
       <c r="C10" s="21"/>
     </row>
-    <row r="11" spans="1:4" s="18" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="18" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>287</v>
       </c>
@@ -4489,17 +4725,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
@@ -4513,7 +4751,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>371</v>
       </c>
@@ -4523,7 +4761,7 @@
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>300</v>
       </c>
@@ -4537,7 +4775,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="132" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="132" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>296</v>
       </c>
@@ -4549,7 +4787,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="63.5" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>372</v>
       </c>
@@ -4591,21 +4829,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.625" customWidth="1"/>
-    <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.375" customWidth="1"/>
-    <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.58203125" customWidth="1"/>
+    <col min="2" max="2" width="27.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.75" customWidth="1"/>
-    <col min="8" max="8" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.08203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
     <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.875" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="28" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>158</v>
       </c>
@@ -4642,7 +4880,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -4653,7 +4891,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -4699,13 +4937,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>158</v>
       </c>
@@ -4716,7 +4954,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -4727,7 +4965,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -4738,7 +4976,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -4749,7 +4987,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -4760,7 +4998,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>200</v>
       </c>
@@ -4771,7 +5009,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>235</v>
       </c>
@@ -4782,7 +5020,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -4793,7 +5031,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -4804,7 +5042,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -4815,7 +5053,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
@@ -4826,7 +5064,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -4837,7 +5075,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
@@ -4848,7 +5086,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -4859,7 +5097,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>247</v>
       </c>
@@ -4870,7 +5108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>248</v>
       </c>
@@ -4881,7 +5119,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>249</v>
       </c>
@@ -4892,7 +5130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>250</v>
       </c>
@@ -4903,7 +5141,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>251</v>
       </c>
@@ -4914,7 +5152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>252</v>
       </c>
@@ -4925,7 +5163,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>253</v>
       </c>
@@ -4936,7 +5174,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>254</v>
       </c>
@@ -4947,7 +5185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>255</v>
       </c>
@@ -4958,7 +5196,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>256</v>
       </c>
@@ -4969,7 +5207,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>257</v>
       </c>
@@ -4980,7 +5218,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>258</v>
       </c>
@@ -4991,7 +5229,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>259</v>
       </c>
@@ -5002,7 +5240,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>260</v>
       </c>
@@ -5013,7 +5251,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>261</v>
       </c>
@@ -5024,7 +5262,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>262</v>
       </c>
@@ -5035,7 +5273,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" s="11" customFormat="1" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
         <v>263</v>
       </c>
@@ -5046,7 +5284,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -5057,7 +5295,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -5119,13 +5357,13 @@
       <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>158</v>
       </c>
@@ -5136,67 +5374,67 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -5252,13 +5490,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>158</v>
       </c>
@@ -5269,112 +5507,112 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>263</v>
       </c>

</xml_diff>